<commit_message>
Published state of ETDataset for deploy January 2024
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/buildings/buildings_cooling_collective_heatpump_water_water_ts_electricity.converter.xlsx
+++ b/nodes_source_analyses/energy/buildings/buildings_cooling_collective_heatpump_water_water_ts_electricity.converter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11210"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/buildings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/nodes_source_analyses/energy/buildings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D5739C-7C29-D546-BCDF-765A0BE6C265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E77CFF-F95E-D44E-B055-1A69DC089CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="17500" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -21,7 +21,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="exchange_rate_2011_2010" localSheetId="4">#REF!</definedName>
@@ -47,7 +46,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -58,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
   <si>
     <t>Source</t>
   </si>
@@ -99,9 +103,6 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Land use of plant in NL</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -159,19 +160,7 @@
     <t>free_co2_factor</t>
   </si>
   <si>
-    <t>forecasting_error</t>
-  </si>
-  <si>
-    <t>land_use_per_unit</t>
-  </si>
-  <si>
     <t>takes_part_in_ets</t>
-  </si>
-  <si>
-    <t>part_load_efficiency_penalty</t>
-  </si>
-  <si>
-    <t>part_load_operating_point</t>
   </si>
   <si>
     <t>electricity_output_capacity</t>
@@ -368,21 +357,6 @@
     <t>Technical</t>
   </si>
   <si>
-    <t>hours_prep_nl</t>
-  </si>
-  <si>
-    <t>hours_prod_nl</t>
-  </si>
-  <si>
-    <t>hours_place_nl</t>
-  </si>
-  <si>
-    <t>hours_maint_nl</t>
-  </si>
-  <si>
-    <t>hours_remov_nl</t>
-  </si>
-  <si>
     <r>
       <t>euro</t>
     </r>
@@ -549,7 +523,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1341,7 +1315,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1356,45 +1330,43 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1411,137 +1383,137 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="26" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="27" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="27" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="19" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="19" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="14" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="15" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="26" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1554,7 +1526,7 @@
     <xf numFmtId="0" fontId="28" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1569,13 +1541,6 @@
     <xf numFmtId="0" fontId="28" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="27" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="26" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="256">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1898,7 +1863,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover Sheet"/>
@@ -2005,27 +1970,6 @@
       <sheetData sheetId="45" refreshError="1"/>
       <sheetData sheetId="46" refreshError="1"/>
       <sheetData sheetId="47" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover sheet"/>
-      <sheetName val="Dashboard"/>
-      <sheetName val="Research data"/>
-      <sheetName val="Sources"/>
-      <sheetName val="Notes"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2360,23 +2304,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="26" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="25" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="18" customWidth="1"/>
     <col min="3" max="3" width="55.1640625" style="18" customWidth="1"/>
     <col min="4" max="16384" width="10.6640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="24" customFormat="1">
-      <c r="A1" s="22"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+    <row r="1" spans="1:3" s="23" customFormat="1">
+      <c r="A1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:3" ht="21">
       <c r="A2" s="1"/>
-      <c r="B2" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="25"/>
+      <c r="B2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1"/>
@@ -2386,28 +2330,28 @@
     <row r="4" spans="1:3">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2422,106 +2366,106 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1"/>
-      <c r="B9" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="81"/>
+      <c r="B9" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1"/>
-      <c r="B10" s="82"/>
-      <c r="C10" s="83"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="78"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1"/>
-      <c r="B11" s="82" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="84" t="s">
-        <v>62</v>
+      <c r="B11" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" thickBot="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="82"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" thickBot="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="85" t="s">
-        <v>64</v>
+      <c r="B13" s="77"/>
+      <c r="C13" s="80" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="83" t="s">
-        <v>65</v>
+      <c r="B14" s="77"/>
+      <c r="C14" s="78" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="83"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="78"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1"/>
-      <c r="B16" s="82" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="86" t="s">
-        <v>67</v>
+      <c r="B16" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="81" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="87" t="s">
-        <v>68</v>
+      <c r="B17" s="77"/>
+      <c r="C17" s="82" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="88" t="s">
-        <v>69</v>
+      <c r="B18" s="77"/>
+      <c r="C18" s="83" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="89" t="s">
-        <v>70</v>
+      <c r="B19" s="77"/>
+      <c r="C19" s="84" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="91" t="s">
-        <v>71</v>
+      <c r="B20" s="85"/>
+      <c r="C20" s="86" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1"/>
-      <c r="B21" s="90"/>
-      <c r="C21" s="92" t="s">
-        <v>72</v>
+      <c r="B21" s="85"/>
+      <c r="C21" s="87" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1"/>
-      <c r="B22" s="90"/>
-      <c r="C22" s="93" t="s">
-        <v>73</v>
+      <c r="B22" s="85"/>
+      <c r="C22" s="88" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" s="90"/>
-      <c r="C23" s="94" t="s">
-        <v>74</v>
+      <c r="B23" s="85"/>
+      <c r="C23" s="89" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2535,64 +2479,50 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:K43"/>
+  <dimension ref="B2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="34" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" style="34" customWidth="1"/>
-    <col min="3" max="3" width="46" style="34" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="34" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="34" customWidth="1"/>
-    <col min="6" max="6" width="4.5" style="34" customWidth="1"/>
-    <col min="7" max="7" width="45" style="34" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" style="34" customWidth="1"/>
-    <col min="9" max="9" width="46.1640625" style="34" customWidth="1"/>
-    <col min="10" max="10" width="5.5" style="34" customWidth="1"/>
-    <col min="11" max="16384" width="10.6640625" style="34"/>
+    <col min="1" max="1" width="3.33203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="46" style="31" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="31" customWidth="1"/>
+    <col min="6" max="6" width="4.5" style="31" customWidth="1"/>
+    <col min="7" max="7" width="45" style="31" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" style="31" customWidth="1"/>
+    <col min="9" max="9" width="46.1640625" style="31" customWidth="1"/>
+    <col min="10" max="10" width="5.5" style="31" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-    </row>
-    <row r="2" spans="2:11">
-      <c r="B2" s="130" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-    </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="133"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-    </row>
-    <row r="4" spans="2:11" ht="38" customHeight="1">
-      <c r="B4" s="136"/>
-      <c r="C4" s="137"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-    </row>
-    <row r="5" spans="2:11" ht="17" thickBot="1">
-      <c r="D5" s="32"/>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="35"/>
+    <row r="2" spans="2:10">
+      <c r="B2" s="126" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="128"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="129"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="131"/>
+    </row>
+    <row r="4" spans="2:10" ht="38" customHeight="1">
+      <c r="B4" s="132"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="134"/>
+    </row>
+    <row r="5" spans="2:10" ht="17" thickBot="1"/>
+    <row r="6" spans="2:10">
+      <c r="B6" s="33"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -2600,14 +2530,14 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
-      <c r="J6" s="36"/>
-    </row>
-    <row r="7" spans="2:11" s="41" customFormat="1" ht="19">
-      <c r="B7" s="95"/>
+      <c r="J6" s="34"/>
+    </row>
+    <row r="7" spans="2:10" s="39" customFormat="1" ht="19">
+      <c r="B7" s="90"/>
       <c r="C7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="91" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="15" t="s">
@@ -2621,667 +2551,476 @@
       <c r="I7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="102"/>
-    </row>
-    <row r="8" spans="2:11" s="41" customFormat="1" ht="19">
+      <c r="J7" s="97"/>
+    </row>
+    <row r="8" spans="2:10" s="39" customFormat="1" ht="19">
       <c r="B8" s="20"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="28"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="42"/>
-    </row>
-    <row r="9" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1">
+      <c r="J8" s="40"/>
+    </row>
+    <row r="9" spans="2:10" s="39" customFormat="1" ht="20" thickBot="1">
       <c r="B9" s="20"/>
       <c r="C9" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="28"/>
+        <v>82</v>
+      </c>
+      <c r="D9" s="27"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="42"/>
-    </row>
-    <row r="10" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1">
+      <c r="J9" s="40"/>
+    </row>
+    <row r="10" spans="2:10" s="39" customFormat="1" ht="20" thickBot="1">
       <c r="B10" s="20"/>
-      <c r="C10" s="129" t="s">
-        <v>100</v>
+      <c r="C10" s="122" t="s">
+        <v>90</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="41">
         <v>0.94760397340000002</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="42"/>
-    </row>
-    <row r="11" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1">
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="40"/>
+    </row>
+    <row r="11" spans="2:10" s="39" customFormat="1" ht="20" thickBot="1">
       <c r="B11" s="20"/>
-      <c r="C11" s="127" t="s">
-        <v>98</v>
+      <c r="C11" s="120" t="s">
+        <v>88</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="41">
         <v>5.2396026630000002E-2</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="42"/>
-    </row>
-    <row r="12" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1">
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="40"/>
+    </row>
+    <row r="12" spans="2:10" s="39" customFormat="1" ht="20" thickBot="1">
       <c r="B12" s="20"/>
-      <c r="C12" s="129" t="s">
-        <v>101</v>
+      <c r="C12" s="122" t="s">
+        <v>91</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="41">
         <v>1</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="42"/>
-    </row>
-    <row r="13" spans="2:11" ht="17" thickBot="1">
-      <c r="B13" s="37"/>
-      <c r="C13" s="33" t="s">
-        <v>31</v>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="40"/>
+    </row>
+    <row r="13" spans="2:10" ht="17" thickBot="1">
+      <c r="B13" s="35"/>
+      <c r="C13" s="32" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="41">
         <v>0</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="103"/>
-      <c r="K13" s="32"/>
-    </row>
-    <row r="14" spans="2:11" ht="17" thickBot="1">
-      <c r="B14" s="37"/>
-      <c r="C14" s="33" t="s">
-        <v>33</v>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="98"/>
+    </row>
+    <row r="14" spans="2:10" ht="17" thickBot="1">
+      <c r="B14" s="35"/>
+      <c r="C14" s="113" t="s">
+        <v>84</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="42">
+        <v>2190</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="98"/>
+    </row>
+    <row r="15" spans="2:10" ht="17" thickBot="1">
+      <c r="B15" s="35"/>
+      <c r="C15" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="42">
         <v>0</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="103"/>
-      <c r="K14" s="32"/>
-    </row>
-    <row r="15" spans="2:11" ht="17" thickBot="1">
-      <c r="B15" s="37"/>
-      <c r="C15" s="120" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="44">
-        <v>2190</v>
-      </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="103"/>
-      <c r="K15" s="32"/>
-    </row>
-    <row r="16" spans="2:11" ht="17" thickBot="1">
-      <c r="B16" s="37"/>
-      <c r="C16" s="33" t="s">
-        <v>36</v>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="32"/>
+      <c r="I15" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="98"/>
+    </row>
+    <row r="16" spans="2:10" ht="17" thickBot="1">
+      <c r="B16" s="35"/>
+      <c r="C16" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="44">
-        <v>0</v>
-      </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="103"/>
-      <c r="K16" s="32"/>
-    </row>
-    <row r="17" spans="2:11" ht="17" thickBot="1">
-      <c r="B17" s="37"/>
-      <c r="C17" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="44">
-        <v>0</v>
-      </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="103"/>
-      <c r="K17" s="32"/>
-    </row>
-    <row r="18" spans="2:11" ht="17" thickBot="1">
-      <c r="B18" s="37"/>
-      <c r="C18" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="44">
-        <v>0</v>
-      </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="33"/>
-      <c r="I18" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="103"/>
-    </row>
-    <row r="19" spans="2:11" ht="17" thickBot="1">
-      <c r="B19" s="37"/>
-      <c r="C19" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="43">
+        <v>53</v>
+      </c>
+      <c r="E16" s="41">
         <f>'Research data'!G6</f>
         <v>2.25</v>
       </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" s="33"/>
-      <c r="I19" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="103"/>
-    </row>
-    <row r="20" spans="2:11">
-      <c r="B20" s="37"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="103"/>
-    </row>
-    <row r="21" spans="2:11">
-      <c r="B21" s="37"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="103"/>
-    </row>
-    <row r="22" spans="2:11" ht="17" thickBot="1">
-      <c r="B22" s="37"/>
-      <c r="C22" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="98"/>
-      <c r="E22" s="99"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="103"/>
-    </row>
-    <row r="23" spans="2:11" ht="17" thickBot="1">
-      <c r="B23" s="37"/>
-      <c r="C23" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="44">
+      <c r="F16" s="32"/>
+      <c r="G16" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="32"/>
+      <c r="I16" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="98"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="35"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="J17" s="98"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="35"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="94"/>
+      <c r="G18" s="56"/>
+      <c r="J18" s="98"/>
+    </row>
+    <row r="19" spans="2:10" ht="17" thickBot="1">
+      <c r="B19" s="35"/>
+      <c r="C19" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="93"/>
+      <c r="E19" s="94"/>
+      <c r="G19" s="56"/>
+      <c r="J19" s="98"/>
+    </row>
+    <row r="20" spans="2:10" ht="17" thickBot="1">
+      <c r="B20" s="35"/>
+      <c r="C20" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="42">
         <f>'Research data'!G14</f>
         <v>953500</v>
       </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33" t="s">
+      <c r="F20" s="32"/>
+      <c r="G20" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="33"/>
-      <c r="I23" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="103"/>
-    </row>
-    <row r="24" spans="2:11" ht="17" thickBot="1">
-      <c r="B24" s="37"/>
-      <c r="C24" s="33" t="s">
-        <v>41</v>
+      <c r="H20" s="32"/>
+      <c r="I20" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="98"/>
+    </row>
+    <row r="21" spans="2:10" ht="17" thickBot="1">
+      <c r="B21" s="35"/>
+      <c r="C21" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="42">
+        <v>0</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="32"/>
+      <c r="I21" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="98"/>
+    </row>
+    <row r="22" spans="2:10" ht="17" thickBot="1">
+      <c r="B22" s="35"/>
+      <c r="C22" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="42">
+        <v>0</v>
+      </c>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="32"/>
+      <c r="I22" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="98"/>
+    </row>
+    <row r="23" spans="2:10" ht="17" thickBot="1">
+      <c r="B23" s="35"/>
+      <c r="C23" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="42">
+        <v>0</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="32"/>
+      <c r="I23" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="98"/>
+    </row>
+    <row r="24" spans="2:10" ht="17" thickBot="1">
+      <c r="B24" s="35"/>
+      <c r="C24" s="32" t="s">
+        <v>38</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="44">
-        <v>0</v>
-      </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="H24" s="33"/>
-      <c r="I24" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="103"/>
-    </row>
-    <row r="25" spans="2:11" ht="17" thickBot="1">
-      <c r="B25" s="37"/>
-      <c r="C25" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="44">
-        <v>0</v>
-      </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="33"/>
-      <c r="I25" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" s="103"/>
-    </row>
-    <row r="26" spans="2:11" ht="17" thickBot="1">
-      <c r="B26" s="37"/>
-      <c r="C26" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="44">
-        <v>0</v>
-      </c>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" s="103"/>
-    </row>
-    <row r="27" spans="2:11" ht="17" thickBot="1">
-      <c r="B27" s="37"/>
-      <c r="C27" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="97">
+        <v>45</v>
+      </c>
+      <c r="E24" s="92">
         <f>'Research data'!G15</f>
         <v>67530</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" s="103"/>
-    </row>
-    <row r="28" spans="2:11" ht="17" thickBot="1">
-      <c r="B28" s="37"/>
-      <c r="C28" s="33" t="s">
+      <c r="F24" s="32"/>
+      <c r="G24" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="32"/>
+      <c r="I24" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="98"/>
+    </row>
+    <row r="25" spans="2:10" ht="17" thickBot="1">
+      <c r="B25" s="35"/>
+      <c r="C25" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="43">
+      <c r="E25" s="41">
         <f>'Research data'!G17</f>
         <v>0</v>
       </c>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H28" s="33"/>
-      <c r="I28" s="79" t="s">
+      <c r="F25" s="32"/>
+      <c r="G25" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="32"/>
+      <c r="I25" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="98"/>
+    </row>
+    <row r="26" spans="2:10" ht="17" thickBot="1">
+      <c r="B26" s="35"/>
+      <c r="C26" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="95">
+        <v>0</v>
+      </c>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="J28" s="103"/>
-    </row>
-    <row r="29" spans="2:11" ht="17" thickBot="1">
-      <c r="B29" s="37"/>
-      <c r="C29" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="100">
+      <c r="H26" s="32"/>
+      <c r="I26" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="98"/>
+    </row>
+    <row r="27" spans="2:10" ht="17" thickBot="1">
+      <c r="B27" s="35"/>
+      <c r="C27" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="41">
+        <v>0.04</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="32"/>
+      <c r="I27" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="J27" s="98"/>
+    </row>
+    <row r="28" spans="2:10" ht="17" thickBot="1">
+      <c r="B28" s="35"/>
+      <c r="C28" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="42">
         <v>0</v>
       </c>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="33"/>
-      <c r="I29" s="110" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" s="103"/>
-    </row>
-    <row r="30" spans="2:11" ht="17" thickBot="1">
-      <c r="B30" s="37"/>
-      <c r="C30" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="43">
-        <v>0.04</v>
-      </c>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" s="33"/>
-      <c r="I30" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="J30" s="103"/>
-    </row>
-    <row r="31" spans="2:11" ht="17" thickBot="1">
-      <c r="B31" s="37"/>
-      <c r="C31" s="33" t="s">
-        <v>35</v>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="98"/>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="35"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="96"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="J29" s="98"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="35"/>
+      <c r="C30" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="93"/>
+      <c r="E30" s="96"/>
+      <c r="J30" s="98"/>
+    </row>
+    <row r="31" spans="2:10" ht="17" thickBot="1">
+      <c r="B31" s="35"/>
+      <c r="C31" s="118" t="s">
+        <v>41</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="44">
+        <v>1</v>
+      </c>
+      <c r="E31" s="92">
+        <f>'Research data'!G10</f>
         <v>0</v>
       </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J31" s="103"/>
-    </row>
-    <row r="32" spans="2:11">
-      <c r="B32" s="37"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="103"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="32"/>
+      <c r="I31" s="106" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="98"/>
+    </row>
+    <row r="32" spans="2:10" ht="17" thickBot="1">
+      <c r="B32" s="35"/>
+      <c r="C32" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="42">
+        <f>'Research data'!G11</f>
+        <v>15</v>
+      </c>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="32"/>
+      <c r="I32" s="107" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="98"/>
     </row>
     <row r="33" spans="2:10" ht="17" thickBot="1">
-      <c r="B33" s="37"/>
-      <c r="C33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="98"/>
-      <c r="E33" s="101"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="42">
+        <v>0</v>
+      </c>
       <c r="F33" s="32"/>
       <c r="G33" s="32"/>
       <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="103"/>
-    </row>
-    <row r="34" spans="2:10" ht="17" thickBot="1">
-      <c r="B34" s="37"/>
-      <c r="C34" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="44">
-        <f>'Research data'!G9</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="33"/>
-      <c r="I34" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J34" s="103"/>
-    </row>
-    <row r="35" spans="2:10" ht="17" thickBot="1">
-      <c r="B35" s="37"/>
-      <c r="C35" s="125" t="s">
+      <c r="I33" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35" s="97">
-        <f>'Research data'!G10</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="H35" s="33"/>
-      <c r="I35" s="112" t="s">
-        <v>51</v>
-      </c>
-      <c r="J35" s="103"/>
-    </row>
-    <row r="36" spans="2:10" ht="17" thickBot="1">
-      <c r="B36" s="37"/>
-      <c r="C36" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="44">
-        <f>'Research data'!G11</f>
-        <v>15</v>
-      </c>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" s="33"/>
-      <c r="I36" s="113" t="s">
-        <v>51</v>
-      </c>
-      <c r="J36" s="103"/>
-    </row>
-    <row r="37" spans="2:10" ht="17" thickBot="1">
-      <c r="B37" s="37"/>
-      <c r="C37" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="44">
-        <v>0</v>
-      </c>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="121" t="s">
-        <v>51</v>
-      </c>
-      <c r="J37" s="103"/>
-    </row>
-    <row r="38" spans="2:10" ht="17" thickBot="1">
-      <c r="B38" s="37"/>
-      <c r="C38" s="116" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="97">
-        <v>6</v>
-      </c>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J38" s="103"/>
-    </row>
-    <row r="39" spans="2:10" ht="17" thickBot="1">
-      <c r="B39" s="37"/>
-      <c r="C39" s="116" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="97">
-        <v>0</v>
-      </c>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J39" s="103"/>
-    </row>
-    <row r="40" spans="2:10" ht="17" thickBot="1">
-      <c r="B40" s="37"/>
-      <c r="C40" s="116" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="97">
-        <v>158410</v>
-      </c>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J40" s="103"/>
-    </row>
-    <row r="41" spans="2:10" ht="17" thickBot="1">
-      <c r="B41" s="37"/>
-      <c r="C41" s="116" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="97">
-        <v>21700</v>
-      </c>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J41" s="103"/>
-    </row>
-    <row r="42" spans="2:10" ht="17" thickBot="1">
-      <c r="B42" s="37"/>
-      <c r="C42" s="116" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="97">
-        <v>40</v>
-      </c>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="J42" s="103"/>
-    </row>
-    <row r="43" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B43" s="38"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="40"/>
+      <c r="J33" s="98"/>
+    </row>
+    <row r="34" spans="2:10" ht="20" customHeight="1" thickBot="1">
+      <c r="B34" s="36"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3305,198 +3044,197 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="3.5" style="60" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="60" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="60" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="60" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="60" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="60" customWidth="1"/>
-    <col min="8" max="8" width="4" style="60" customWidth="1"/>
-    <col min="9" max="9" width="16" style="60" customWidth="1"/>
-    <col min="10" max="10" width="3" style="61" customWidth="1"/>
-    <col min="11" max="11" width="60" style="60" customWidth="1"/>
-    <col min="12" max="16384" width="10.6640625" style="60"/>
+    <col min="1" max="2" width="3.5" style="56" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="56" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="56" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="56" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="56" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="56" customWidth="1"/>
+    <col min="8" max="8" width="4" style="56" customWidth="1"/>
+    <col min="9" max="9" width="16" style="56" customWidth="1"/>
+    <col min="10" max="10" width="3" style="57" customWidth="1"/>
+    <col min="11" max="11" width="60" style="56" customWidth="1"/>
+    <col min="12" max="16384" width="10.6640625" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1"/>
     <row r="2" spans="2:11">
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="63"/>
-    </row>
-    <row r="3" spans="2:11" s="21" customFormat="1">
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="59"/>
+    </row>
+    <row r="3" spans="2:11" s="14" customFormat="1">
       <c r="B3" s="20"/>
-      <c r="C3" s="108" t="s">
-        <v>77</v>
+      <c r="C3" s="103" t="s">
+        <v>72</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="108" t="s">
+      <c r="F3" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="108" t="s">
+      <c r="G3" s="103" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="54"/>
+      <c r="K3" s="103" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="61"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="2:11" ht="17" thickBot="1">
+      <c r="B5" s="61"/>
+      <c r="C5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108" t="s">
-        <v>106</v>
-      </c>
-      <c r="J3" s="58"/>
-      <c r="K3" s="108" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="65"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="2:11" ht="17" thickBot="1">
-      <c r="B5" s="65"/>
-      <c r="C5" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="59"/>
+      <c r="K5" s="55"/>
     </row>
     <row r="6" spans="2:11" ht="17" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="122" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="123">
+      <c r="B6" s="61"/>
+      <c r="C6" s="115" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="116">
         <f>Notes!E6/1000</f>
         <v>2.25</v>
       </c>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="59"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="55"/>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="65"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="109"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="55"/>
     </row>
     <row r="8" spans="2:11" ht="17" thickBot="1">
-      <c r="B8" s="65"/>
-      <c r="C8" s="29" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="30"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="2:11" ht="17" thickBot="1">
-      <c r="B9" s="65"/>
-      <c r="C9" s="75" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="124" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="118">
+      <c r="G9" s="111">
         <f>ROUND(0,0)</f>
         <v>0</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
-      <c r="K9" s="30"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="2:11" ht="17" thickBot="1">
-      <c r="B10" s="65"/>
-      <c r="C10" s="75" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="69" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="118">
+      <c r="G10" s="111">
         <f>ROUND(0,0)</f>
         <v>0</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
-      <c r="K10" s="30"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="2:11" ht="17" thickBot="1">
-      <c r="B11" s="65"/>
-      <c r="C11" s="75" t="s">
+      <c r="B11" s="61"/>
+      <c r="C11" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="69" t="s">
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="118">
+      <c r="G11" s="111">
         <f>ROUND(15,0)</f>
         <v>15</v>
       </c>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="114"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="108"/>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="65"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="59"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="55"/>
     </row>
     <row r="13" spans="2:11" ht="17" thickBot="1">
-      <c r="B13" s="65"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -3505,104 +3243,104 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
-      <c r="K13" s="59"/>
+      <c r="K13" s="55"/>
     </row>
     <row r="14" spans="2:11" ht="17" thickBot="1">
-      <c r="B14" s="65"/>
-      <c r="C14" s="104" t="s">
-        <v>81</v>
+      <c r="B14" s="61"/>
+      <c r="C14" s="99" t="s">
+        <v>76</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="104" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="78">
+      <c r="F14" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="73">
         <f>I14</f>
         <v>953500</v>
       </c>
       <c r="H14" s="12"/>
-      <c r="I14" s="78">
+      <c r="I14" s="73">
         <f>Notes!E12</f>
         <v>953500</v>
       </c>
-      <c r="J14" s="71"/>
-      <c r="K14" s="115"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="109"/>
     </row>
     <row r="15" spans="2:11" ht="17" thickBot="1">
-      <c r="B15" s="65"/>
-      <c r="C15" s="111" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="117" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" s="126">
+      <c r="B15" s="61"/>
+      <c r="C15" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="110" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="119">
         <f>ROUND((G16*G6*1000),2)</f>
         <v>67530</v>
       </c>
       <c r="H15" s="12"/>
-      <c r="I15" s="128"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="119"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="112"/>
     </row>
     <row r="16" spans="2:11" ht="17" thickBot="1">
-      <c r="B16" s="65"/>
-      <c r="C16" s="104" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="106" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="142">
+      <c r="B16" s="61"/>
+      <c r="C16" s="99" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="101" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="124">
         <v>30.013332999999999</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="143" t="s">
-        <v>114</v>
+      <c r="J16" s="67"/>
+      <c r="K16" s="125" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="17" thickBot="1">
-      <c r="B17" s="65"/>
-      <c r="C17" s="111" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="69" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="78">
+      <c r="B17" s="61"/>
+      <c r="C17" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="73">
         <v>0</v>
       </c>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="115"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="109"/>
     </row>
     <row r="18" spans="2:11" ht="17" thickBot="1">
-      <c r="B18" s="65"/>
-      <c r="C18" s="104" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="105" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="78">
+      <c r="B18" s="61"/>
+      <c r="C18" s="99" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="100" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="73">
         <v>0</v>
       </c>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="30"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3623,83 +3361,73 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="45" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="45" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="45" customWidth="1"/>
-    <col min="4" max="4" width="3.1640625" style="45" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="45" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="45" customWidth="1"/>
-    <col min="7" max="9" width="12.1640625" style="45" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="46" customWidth="1"/>
-    <col min="11" max="11" width="66" style="45" customWidth="1"/>
-    <col min="12" max="16384" width="33.1640625" style="45"/>
+    <col min="1" max="1" width="3.33203125" style="43" customWidth="1"/>
+    <col min="2" max="2" width="3.5" style="43" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="43" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" style="43" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="43" customWidth="1"/>
+    <col min="7" max="9" width="12.1640625" style="43" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="44" customWidth="1"/>
+    <col min="11" max="11" width="66" style="43" customWidth="1"/>
+    <col min="12" max="16384" width="33.1640625" style="43"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1"/>
     <row r="2" spans="2:11">
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="48"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="50"/>
-      <c r="C3" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="50"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="53"/>
+      <c r="B4" s="48"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="55"/>
-      <c r="C5" s="56" t="s">
+      <c r="B5" s="51"/>
+      <c r="C5" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="I5" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="K5" s="56" t="s">
-        <v>14</v>
+      <c r="H5" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="52" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3721,136 +3449,134 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="45" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="45" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="45" customWidth="1"/>
-    <col min="4" max="4" width="3.1640625" style="45" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="45" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="45" customWidth="1"/>
-    <col min="7" max="9" width="12.1640625" style="45" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="46" customWidth="1"/>
-    <col min="11" max="11" width="66" style="45" customWidth="1"/>
-    <col min="12" max="16384" width="33.1640625" style="45"/>
+    <col min="1" max="1" width="3.33203125" style="43" customWidth="1"/>
+    <col min="2" max="2" width="3.5" style="43" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="43" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" style="43" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="43" customWidth="1"/>
+    <col min="7" max="9" width="12.1640625" style="43" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="44" customWidth="1"/>
+    <col min="11" max="11" width="66" style="43" customWidth="1"/>
+    <col min="12" max="16384" width="33.1640625" style="43"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1"/>
     <row r="2" spans="2:11">
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="48"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="50"/>
-      <c r="C3" s="139"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="139"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="139"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="50"/>
+      <c r="B4" s="48"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="55"/>
-      <c r="C5" s="56" t="s">
+      <c r="B5" s="51"/>
+      <c r="C5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="56"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="52"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="53"/>
-      <c r="C6" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="53">
+      <c r="C6" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="49"/>
+      <c r="E6" s="43">
         <v>2250</v>
       </c>
-      <c r="F6" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="51"/>
+      <c r="F6" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="49"/>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="53"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="51"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="49"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="C8" s="139" t="s">
-        <v>112</v>
+      <c r="C8" s="49" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="2:11">
-      <c r="C10" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="45">
+      <c r="C10" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="43">
         <v>8500</v>
       </c>
-      <c r="F10" s="45" t="s">
-        <v>108</v>
+      <c r="F10" s="43" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="C11" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" s="45">
+      <c r="C11" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="43">
         <v>420</v>
       </c>
-      <c r="F11" s="45" t="s">
-        <v>110</v>
+      <c r="F11" s="43" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="2:11">
-      <c r="C12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="45">
+      <c r="C12" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="43">
         <f>E10+E11*E6</f>
         <v>953500</v>
       </c>
-      <c r="F12" s="45" t="s">
-        <v>111</v>
+      <c r="F12" s="43" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="3:5">
-      <c r="C17" s="139"/>
+      <c r="C17" s="49"/>
     </row>
     <row r="19" spans="3:5">
-      <c r="E19" s="141"/>
+      <c r="E19" s="123"/>
     </row>
     <row r="20" spans="3:5">
-      <c r="E20" s="141"/>
+      <c r="E20" s="123"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>